<commit_message>
envio de dados configurado
</commit_message>
<xml_diff>
--- a/alvoss.xlsx
+++ b/alvoss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisRibeiro\Documents\phishing_via_email\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8A3B9E-6984-4F86-A9CA-1F43EDC0B858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E5EBEF-CDFF-4A5D-A855-65F469B1FD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4815" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>nome</t>
   </si>
@@ -37,13 +37,25 @@
   </si>
   <si>
     <t>logxpbr@gmail.com</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>luisclr.contato@gmail.com</t>
+  </si>
+  <si>
+    <t>contato.jordaquino@gmail.com</t>
+  </si>
+  <si>
+    <t>Jordan Aquino</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +67,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,9 +101,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -365,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,11 +410,32 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{440FA85A-6AB5-4CF4-BF4A-51392CCD32A6}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{E6261596-6CC7-4FF3-89DF-198DF5FE84B8}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{7F84A1F3-0AE7-48AC-9C4D-4B8B0772B456}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>